<commit_message>
feat: :sparkles: refactoring code from arduino to esp32.
All the changes reflects it.
</commit_message>
<xml_diff>
--- a/EletronicaChallenge.xlsx
+++ b/EletronicaChallenge.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leand\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leandroluna/Documents/Github/ChallengeToledo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11A3C8F6-A20D-4FF8-933F-F266F8A9B7C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77D303FB-58E8-7842-A1AE-F961CB03CD04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{5E96AFFE-0A04-4B47-AFB6-2D8EE016FDF0}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{5E96AFFE-0A04-4B47-AFB6-2D8EE016FDF0}"/>
   </bookViews>
   <sheets>
-    <sheet name="Lista de componentes - V2" sheetId="1" r:id="rId1"/>
-    <sheet name="Conexões - V1" sheetId="2" r:id="rId2"/>
+    <sheet name="Lista de componentes - V3" sheetId="1" r:id="rId1"/>
+    <sheet name="Conexões - V2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -102,9 +102,6 @@
     <t>https://tinyurl.com/29u4w6yx</t>
   </si>
   <si>
-    <t>Arduino Uno R3</t>
-  </si>
-  <si>
     <t>https://tinyurl.com/ycxjwjnb</t>
   </si>
   <si>
@@ -165,12 +162,6 @@
     <t>https://tinyurl.com/yttc3hhv</t>
   </si>
   <si>
-    <t>D2</t>
-  </si>
-  <si>
-    <t>A0</t>
-  </si>
-  <si>
     <t>3.3V</t>
   </si>
   <si>
@@ -189,24 +180,9 @@
     <t>SDA</t>
   </si>
   <si>
-    <t>5V (Arduino?)</t>
-  </si>
-  <si>
-    <t>A4</t>
-  </si>
-  <si>
-    <t>A5</t>
-  </si>
-  <si>
     <t>LED Difuso (Vermelho)</t>
   </si>
   <si>
-    <t>D4 (Utilizar resistor de 1K)</t>
-  </si>
-  <si>
-    <t>D5 (Utilizar resistor de 1K)</t>
-  </si>
-  <si>
     <t>LED Difuso (Verde)</t>
   </si>
   <si>
@@ -216,19 +192,43 @@
     <t>TRIG</t>
   </si>
   <si>
-    <t>D11</t>
-  </si>
-  <si>
-    <t>D12</t>
-  </si>
-  <si>
-    <t>D3</t>
-  </si>
-  <si>
     <t>Pinagem</t>
   </si>
   <si>
     <t>Total desconsiderando o frete</t>
+  </si>
+  <si>
+    <t>D34</t>
+  </si>
+  <si>
+    <t>D13</t>
+  </si>
+  <si>
+    <t>D32</t>
+  </si>
+  <si>
+    <t>D33 (Utilizar resistor de 330ohm)</t>
+  </si>
+  <si>
+    <t>D25 (Utilizar resistor de 330ohm)</t>
+  </si>
+  <si>
+    <t>D26</t>
+  </si>
+  <si>
+    <t>D27</t>
+  </si>
+  <si>
+    <t>D21</t>
+  </si>
+  <si>
+    <t>D22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESP32 </t>
+  </si>
+  <si>
+    <t>5V (ESP32)</t>
   </si>
 </sst>
 </file>
@@ -236,8 +236,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="[$R$-416]\ #,##0.00"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="[$R$-416]\ #,##0.00"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -476,11 +476,11 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -488,58 +488,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="1" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -547,7 +541,7 @@
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="2" builtinId="5"/>
+    <cellStyle name="Per cent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -862,20 +856,20 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="65.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -888,19 +882,19 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>21</v>
+        <v>62</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -908,19 +902,19 @@
       <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="7">
-        <v>59.76</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E2" s="5">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
@@ -928,19 +922,19 @@
       <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="5">
         <v>0.28000000000000003</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F3" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
@@ -948,14 +942,14 @@
       <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="5">
         <v>2.76</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -968,19 +962,19 @@
       <c r="D5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="5">
         <v>14.94</v>
       </c>
-      <c r="F5" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" s="2">
         <v>2</v>
@@ -988,19 +982,19 @@
       <c r="D6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="5">
         <v>0.56000000000000005</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="2">
         <v>1</v>
@@ -1008,19 +1002,19 @@
       <c r="D7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="5">
         <v>11.99</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" s="2">
         <v>1</v>
@@ -1028,19 +1022,19 @@
       <c r="D8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="5">
         <v>11.61</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F8" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" s="2">
         <v>2</v>
@@ -1048,19 +1042,19 @@
       <c r="D9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="5">
         <v>0.12</v>
       </c>
-      <c r="F9" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F9" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>4</v>
@@ -1068,19 +1062,19 @@
       <c r="D10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="5">
         <v>14.16</v>
       </c>
-      <c r="F10" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F10" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>4</v>
@@ -1088,19 +1082,19 @@
       <c r="D11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="5">
         <v>6.56</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F11" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12" s="2">
         <v>1</v>
@@ -1108,44 +1102,44 @@
       <c r="D12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="5">
         <v>11.2</v>
       </c>
-      <c r="F12" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+      <c r="F12" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <v>1</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="5">
         <v>10.5</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D14" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="E14" s="19">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D14" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="12">
         <f>SUM(E2:E13)</f>
-        <v>144.44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D15" s="4"/>
+        <v>118.88000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D15" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1171,216 +1165,216 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C1" s="18"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="9" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="16"/>
+      <c r="B3" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="15"/>
+      <c r="B5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="16"/>
+      <c r="B6" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="15"/>
+      <c r="B8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="15"/>
+      <c r="B9" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="11"/>
-      <c r="B3" s="12" t="s">
+      <c r="C9" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="16"/>
+      <c r="B10" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C10" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="15" t="s">
+      <c r="C11" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="16"/>
+      <c r="B12" s="8" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="11"/>
-      <c r="B6" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C6" s="13" t="s">
+      <c r="C12" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="16"/>
+      <c r="B14" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="15"/>
+      <c r="B16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="15"/>
+      <c r="B17" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="16"/>
+      <c r="B18" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="15"/>
+      <c r="B20" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="11"/>
-      <c r="B10" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="11"/>
-      <c r="B12" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" s="13" t="s">
+      <c r="C20" s="10" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="11"/>
-      <c r="B14" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="11"/>
-      <c r="B18" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="11"/>
-      <c r="B21" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>50</v>
+    <row r="21" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="16"/>
+      <c r="B21" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: :sparkles: add multi cell util
</commit_message>
<xml_diff>
--- a/EletronicaChallenge.xlsx
+++ b/EletronicaChallenge.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leandroluna/Documents/Github/ChallengeToledo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leand\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77D303FB-58E8-7842-A1AE-F961CB03CD04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92BC9728-F59D-4C0B-90B2-EC80C319202C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{5E96AFFE-0A04-4B47-AFB6-2D8EE016FDF0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5E96AFFE-0A04-4B47-AFB6-2D8EE016FDF0}"/>
   </bookViews>
   <sheets>
-    <sheet name="Lista de componentes - V3" sheetId="1" r:id="rId1"/>
-    <sheet name="Conexões - V2" sheetId="2" r:id="rId2"/>
+    <sheet name="Lista de componentes - V5" sheetId="1" r:id="rId1"/>
+    <sheet name="Conexões - V4" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="76">
   <si>
     <t>Enumerador</t>
   </si>
@@ -78,15 +78,6 @@
     <t>Reúne os componentes e as conexões com o microcontrolador</t>
   </si>
   <si>
-    <t>Alterna modo de abrir e fechar a cancela</t>
-  </si>
-  <si>
-    <t>Display SSD1306 128x32</t>
-  </si>
-  <si>
-    <t>Apresenta o peso, a distância e o estado do portão (aberto ou fechado)</t>
-  </si>
-  <si>
     <t>Fonte ajustável MB102</t>
   </si>
   <si>
@@ -105,21 +96,12 @@
     <t>https://tinyurl.com/ycxjwjnb</t>
   </si>
   <si>
-    <t>Push Button</t>
-  </si>
-  <si>
-    <t>https://tinyurl.com/2p97anph</t>
-  </si>
-  <si>
     <t>Potenciômetro 10KΩ</t>
   </si>
   <si>
     <t>https://tinyurl.com/2mvx7ckn</t>
   </si>
   <si>
-    <t>https://tinyurl.com/mrx9ata3</t>
-  </si>
-  <si>
     <t>LED Difuso</t>
   </si>
   <si>
@@ -180,12 +162,6 @@
     <t>SDA</t>
   </si>
   <si>
-    <t>LED Difuso (Vermelho)</t>
-  </si>
-  <si>
-    <t>LED Difuso (Verde)</t>
-  </si>
-  <si>
     <t>ECHO</t>
   </si>
   <si>
@@ -204,9 +180,6 @@
     <t>D13</t>
   </si>
   <si>
-    <t>D32</t>
-  </si>
-  <si>
     <t>D33 (Utilizar resistor de 330ohm)</t>
   </si>
   <si>
@@ -229,6 +202,69 @@
   </si>
   <si>
     <t>5V (ESP32)</t>
+  </si>
+  <si>
+    <t>RFID-RC522</t>
+  </si>
+  <si>
+    <t>MOSI</t>
+  </si>
+  <si>
+    <t>MISO</t>
+  </si>
+  <si>
+    <t>IRQ</t>
+  </si>
+  <si>
+    <t>RST</t>
+  </si>
+  <si>
+    <t>D18</t>
+  </si>
+  <si>
+    <t>D23</t>
+  </si>
+  <si>
+    <t>D19</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Leitor RFID-RC522</t>
+  </si>
+  <si>
+    <t>Identificação dos caminhões</t>
+  </si>
+  <si>
+    <t>https://tinyurl.com/bp7fehnv</t>
+  </si>
+  <si>
+    <t>LED Difuso (Vermelho - Frente)</t>
+  </si>
+  <si>
+    <t>LED Difuso (Verde - Frente)</t>
+  </si>
+  <si>
+    <t>Servo Motor SG90 (Frente)</t>
+  </si>
+  <si>
+    <t>LED Difuso (Vermelho - Trás)</t>
+  </si>
+  <si>
+    <t>LED Difuso (Verde - Trás)</t>
+  </si>
+  <si>
+    <t>D14 (Utilizar resistor de 330ohm)</t>
+  </si>
+  <si>
+    <t>D12 (Utilizar resistor de 330ohm)</t>
+  </si>
+  <si>
+    <t>Servo Motor SG90 (Trás)</t>
+  </si>
+  <si>
+    <t>D5</t>
   </si>
 </sst>
 </file>
@@ -236,8 +272,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="[$R$-416]\ #,##0.00"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="[$R$-416]\ #,##0.00"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -285,7 +321,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -473,14 +509,66 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -488,13 +576,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -515,12 +600,34 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="16" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -528,6 +635,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -541,7 +651,7 @@
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Per cent" xfId="2" builtinId="5"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -853,23 +963,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16DB31F4-337A-44A2-8F54-CF903EED1856}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="65.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="20" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -882,19 +992,19 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>18</v>
+      <c r="E1" s="18" t="s">
+        <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -902,491 +1012,554 @@
       <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="4">
         <v>34.200000000000003</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F2" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="5">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="E3" s="4">
+        <v>2.76</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C4" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="5">
-        <v>2.76</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="C5" s="2">
         <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="5">
-        <v>14.94</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+      <c r="E5" s="4">
+        <v>11.99</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6" s="2">
         <v>2</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="5">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="E6" s="4">
+        <v>11.61</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C7" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="5">
-        <v>11.99</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0.12</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="2">
-        <v>1</v>
+        <v>29</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="5">
-        <v>11.61</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="E8" s="4">
+        <v>14.16</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="2">
-        <v>2</v>
+        <v>31</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="5">
-        <v>0.12</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="E9" s="4">
+        <v>6.56</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>4</v>
+        <v>33</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="5">
-        <v>14.16</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="E10" s="4">
+        <v>11.2</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="5">
-        <v>6.56</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="E11" s="4">
+        <v>10.5</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="C12" s="2">
         <v>1</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="5">
-        <v>11.2</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
-        <v>12</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="2">
-        <v>1</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="5">
-        <v>10.5</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D14" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="E14" s="12">
-        <f>SUM(E2:E13)</f>
-        <v>118.88000000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D15" s="3"/>
+        <v>65</v>
+      </c>
+      <c r="E12" s="19">
+        <v>34.99</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D13" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="17">
+        <f>SUM(E2:E12)</f>
+        <v>138.65</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{528D3BFB-6302-4333-AF61-574192AC7DF6}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{163CBE85-C187-4DF9-9D64-FEB36BF2E201}"/>
-    <hyperlink ref="F4" r:id="rId3" xr:uid="{62AC7026-C88D-4774-9E77-2E076F277D78}"/>
-    <hyperlink ref="F5" r:id="rId4" xr:uid="{ED12DA98-0674-425A-8564-8977D9C29F94}"/>
-    <hyperlink ref="F6" r:id="rId5" xr:uid="{929B1F67-A872-4C99-B49D-04DEA1A6EF10}"/>
-    <hyperlink ref="F7" r:id="rId6" xr:uid="{B531E9DF-691B-412C-8EFD-8D1A68459FA6}"/>
-    <hyperlink ref="F8" r:id="rId7" xr:uid="{37B59F20-7907-4950-B248-C8B22EADB14E}"/>
-    <hyperlink ref="F9" r:id="rId8" xr:uid="{662E3503-C0A2-424F-82DB-96F697CE52AE}"/>
-    <hyperlink ref="F10" r:id="rId9" xr:uid="{99323563-C228-4D7A-A8D4-F4DF516FBD4C}"/>
-    <hyperlink ref="F11" r:id="rId10" xr:uid="{496BBC37-B6FF-43D4-8A15-88DA8CD31A24}"/>
-    <hyperlink ref="F12" r:id="rId11" xr:uid="{C6F094FC-4A30-43B3-A977-859284AF2B67}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{62AC7026-C88D-4774-9E77-2E076F277D78}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{929B1F67-A872-4C99-B49D-04DEA1A6EF10}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{B531E9DF-691B-412C-8EFD-8D1A68459FA6}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{37B59F20-7907-4950-B248-C8B22EADB14E}"/>
+    <hyperlink ref="F7" r:id="rId6" xr:uid="{662E3503-C0A2-424F-82DB-96F697CE52AE}"/>
+    <hyperlink ref="F8" r:id="rId7" xr:uid="{99323563-C228-4D7A-A8D4-F4DF516FBD4C}"/>
+    <hyperlink ref="F9" r:id="rId8" xr:uid="{496BBC37-B6FF-43D4-8A15-88DA8CD31A24}"/>
+    <hyperlink ref="F10" r:id="rId9" xr:uid="{C6F094FC-4A30-43B3-A977-859284AF2B67}"/>
+    <hyperlink ref="F12" r:id="rId10" xr:uid="{B76E3EE7-B20F-4FCC-9E2F-E2B01EFE7E88}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53FAE084-AB77-4E13-B4AD-AFA90B81183D}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.5703125" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="26"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="22"/>
+      <c r="B3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="23"/>
+      <c r="B4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="23"/>
+      <c r="B6" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="23"/>
+      <c r="B8" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="22"/>
+      <c r="B10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="22"/>
+      <c r="B11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="23"/>
+      <c r="B12" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="22"/>
+      <c r="B14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="24"/>
+      <c r="B15" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="18"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
-      <c r="B3" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="15"/>
-      <c r="B5" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="15"/>
-      <c r="B8" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" s="10" t="s">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="22"/>
+      <c r="B17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="22"/>
+      <c r="B18" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="22"/>
+      <c r="B19" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="22"/>
+      <c r="B20" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="14" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="15"/>
-      <c r="B9" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
-      <c r="B10" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
-      <c r="B12" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
-      <c r="B14" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="15"/>
-      <c r="B16" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="10" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="22"/>
+      <c r="B21" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="22"/>
+      <c r="B22" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="15"/>
-      <c r="B17" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="16"/>
-      <c r="B18" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="15"/>
-      <c r="B20" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="16"/>
-      <c r="B21" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>41</v>
+      <c r="C22" s="14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="23"/>
+      <c r="B23" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="23"/>
+      <c r="B25" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="23"/>
+      <c r="B27" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="22"/>
+      <c r="B29" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="23"/>
+      <c r="B30" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A19:A21"/>
+  <mergeCells count="10">
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A16:A23"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A13:A15"/>
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A6"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
refact code and upd eletronic spreedsheet
</commit_message>
<xml_diff>
--- a/EletronicaChallenge.xlsx
+++ b/EletronicaChallenge.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leand\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92BC9728-F59D-4C0B-90B2-EC80C319202C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B8594F8-A42E-4ABC-BFAD-B8283D8BDA9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5E96AFFE-0A04-4B47-AFB6-2D8EE016FDF0}"/>
   </bookViews>
   <sheets>
-    <sheet name="Lista de componentes - V5" sheetId="1" r:id="rId1"/>
-    <sheet name="Conexões - V4" sheetId="2" r:id="rId2"/>
+    <sheet name="Lista de componentes - Final" sheetId="1" r:id="rId1"/>
+    <sheet name="Conexões - Final" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="66">
   <si>
     <t>Enumerador</t>
   </si>
@@ -63,9 +63,6 @@
     <t>Farol (LED vermelho e verde)</t>
   </si>
   <si>
-    <t>Indica posição segura entre o caminhão e a cancela</t>
-  </si>
-  <si>
     <t>Cancela: 0º fechado, 90º aberto</t>
   </si>
   <si>
@@ -78,21 +75,12 @@
     <t>Reúne os componentes e as conexões com o microcontrolador</t>
   </si>
   <si>
-    <t>Fonte ajustável MB102</t>
-  </si>
-  <si>
-    <t>Alimentação externa de 5V</t>
-  </si>
-  <si>
     <t>Preço</t>
   </si>
   <si>
     <t>Link</t>
   </si>
   <si>
-    <t>https://tinyurl.com/29u4w6yx</t>
-  </si>
-  <si>
     <t>https://tinyurl.com/ycxjwjnb</t>
   </si>
   <si>
@@ -111,12 +99,6 @@
     <t>https://tinyurl.com/2c23wu55</t>
   </si>
   <si>
-    <t>Sensor Ultrassônico HCSR-04</t>
-  </si>
-  <si>
-    <t>https://tinyurl.com/ydaypk5b</t>
-  </si>
-  <si>
     <t>Servo Motor SG90</t>
   </si>
   <si>
@@ -162,12 +144,6 @@
     <t>SDA</t>
   </si>
   <si>
-    <t>ECHO</t>
-  </si>
-  <si>
-    <t>TRIG</t>
-  </si>
-  <si>
     <t>Pinagem</t>
   </si>
   <si>
@@ -186,12 +162,6 @@
     <t>D25 (Utilizar resistor de 330ohm)</t>
   </si>
   <si>
-    <t>D26</t>
-  </si>
-  <si>
-    <t>D27</t>
-  </si>
-  <si>
     <t>D21</t>
   </si>
   <si>
@@ -201,9 +171,6 @@
     <t xml:space="preserve">ESP32 </t>
   </si>
   <si>
-    <t>5V (ESP32)</t>
-  </si>
-  <si>
     <t>RFID-RC522</t>
   </si>
   <si>
@@ -265,6 +232,9 @@
   </si>
   <si>
     <t>D5</t>
+  </si>
+  <si>
+    <t>5V</t>
   </si>
 </sst>
 </file>
@@ -628,6 +598,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -639,12 +615,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -963,10 +933,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16DB31F4-337A-44A2-8F54-CF903EED1856}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -993,10 +963,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1004,7 +974,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -1016,7 +986,7 @@
         <v>34.200000000000003</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1024,7 +994,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
@@ -1036,7 +1006,7 @@
         <v>2.76</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1044,7 +1014,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C4" s="2">
         <v>4</v>
@@ -1056,176 +1026,136 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C5" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="4">
-        <v>11.99</v>
+        <v>11.61</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C6" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E6" s="4">
-        <v>11.61</v>
+        <v>0.12</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="2">
+        <v>23</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E7" s="4">
-        <v>0.12</v>
+        <v>14.16</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8" s="4">
-        <v>14.16</v>
+        <v>6.56</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>4</v>
+        <v>27</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E9" s="4">
-        <v>6.56</v>
+        <v>11.2</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="C10" s="2">
         <v>1</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="4">
-        <v>11.2</v>
+        <v>54</v>
+      </c>
+      <c r="E10" s="19">
+        <v>34.99</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="2">
-        <v>1</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="4">
-        <v>10.5</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>11</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C12" s="2">
-        <v>1</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E12" s="19">
-        <v>34.99</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D13" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" s="17">
-        <f>SUM(E2:E12)</f>
-        <v>138.65</v>
+      <c r="D11" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="17">
+        <f>SUM(E2:E10)</f>
+        <v>116.16</v>
       </c>
     </row>
   </sheetData>
@@ -1233,25 +1163,24 @@
     <hyperlink ref="F2" r:id="rId1" xr:uid="{528D3BFB-6302-4333-AF61-574192AC7DF6}"/>
     <hyperlink ref="F3" r:id="rId2" xr:uid="{62AC7026-C88D-4774-9E77-2E076F277D78}"/>
     <hyperlink ref="F4" r:id="rId3" xr:uid="{929B1F67-A872-4C99-B49D-04DEA1A6EF10}"/>
-    <hyperlink ref="F5" r:id="rId4" xr:uid="{B531E9DF-691B-412C-8EFD-8D1A68459FA6}"/>
-    <hyperlink ref="F6" r:id="rId5" xr:uid="{37B59F20-7907-4950-B248-C8B22EADB14E}"/>
-    <hyperlink ref="F7" r:id="rId6" xr:uid="{662E3503-C0A2-424F-82DB-96F697CE52AE}"/>
-    <hyperlink ref="F8" r:id="rId7" xr:uid="{99323563-C228-4D7A-A8D4-F4DF516FBD4C}"/>
-    <hyperlink ref="F9" r:id="rId8" xr:uid="{496BBC37-B6FF-43D4-8A15-88DA8CD31A24}"/>
-    <hyperlink ref="F10" r:id="rId9" xr:uid="{C6F094FC-4A30-43B3-A977-859284AF2B67}"/>
-    <hyperlink ref="F12" r:id="rId10" xr:uid="{B76E3EE7-B20F-4FCC-9E2F-E2B01EFE7E88}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{37B59F20-7907-4950-B248-C8B22EADB14E}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{662E3503-C0A2-424F-82DB-96F697CE52AE}"/>
+    <hyperlink ref="F7" r:id="rId6" xr:uid="{99323563-C228-4D7A-A8D4-F4DF516FBD4C}"/>
+    <hyperlink ref="F8" r:id="rId7" xr:uid="{496BBC37-B6FF-43D4-8A15-88DA8CD31A24}"/>
+    <hyperlink ref="F9" r:id="rId8" xr:uid="{C6F094FC-4A30-43B3-A977-859284AF2B67}"/>
+    <hyperlink ref="F10" r:id="rId9" xr:uid="{B76E3EE7-B20F-4FCC-9E2F-E2B01EFE7E88}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53FAE084-AB77-4E13-B4AD-AFA90B81183D}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1264,302 +1193,263 @@
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" s="26"/>
+      <c r="B1" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="22"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
-        <v>19</v>
+      <c r="A2" s="23" t="s">
+        <v>15</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
+      <c r="A3" s="24"/>
       <c r="B3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="25"/>
+      <c r="B4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="25"/>
+      <c r="B6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="25"/>
+      <c r="B8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="24"/>
+      <c r="B10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="9" t="s">
+    </row>
+    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="26"/>
+      <c r="B11" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="24"/>
+      <c r="B13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="24"/>
+      <c r="B14" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="23"/>
-      <c r="B4" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="23"/>
-      <c r="B6" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="8" t="s">
+      <c r="C14" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="24"/>
+      <c r="B15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="24"/>
+      <c r="B16" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="23"/>
-      <c r="B8" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="8" t="s">
+      <c r="C16" s="14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="24"/>
+      <c r="B17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="24"/>
+      <c r="B18" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="22"/>
-      <c r="B10" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="2" t="s">
+      <c r="C18" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="23"/>
-      <c r="B12" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="22"/>
-      <c r="B14" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="24"/>
-      <c r="B15" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="22"/>
-      <c r="B17" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="14" t="s">
+    </row>
+    <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="25"/>
+      <c r="B19" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="25"/>
+      <c r="B21" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="23" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="22"/>
-      <c r="B18" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="22"/>
-      <c r="B19" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C19" s="14" t="s">
+      <c r="B22" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="25"/>
+      <c r="B23" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="22"/>
-      <c r="B20" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C20" s="14" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="23" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="22"/>
-      <c r="B21" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
-      <c r="B22" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="23"/>
-      <c r="B23" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="21" t="s">
-        <v>70</v>
-      </c>
       <c r="B24" s="5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="23"/>
-      <c r="B25" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="23"/>
-      <c r="B27" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="22"/>
-      <c r="B29" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="23"/>
-      <c r="B30" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>35</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="24"/>
+      <c r="B25" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="25"/>
+      <c r="B26" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="A16:A23"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="A13:A15"/>
+  <mergeCells count="9">
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A12:A19"/>
+    <mergeCell ref="A9:A11"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A20:A21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>